<commit_message>
twwo image constructor created
</commit_message>
<xml_diff>
--- a/Тест_книги.xlsx
+++ b/Тест_книги.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrkhikmatullin/PycharmProjects/imageTemplateGenerating/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CBE08E-6E11-0648-A6E1-0C333A788297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F64FF-C677-9B43-AD1A-778EA407D50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6320" yWindow="3400" windowWidth="28240" windowHeight="17240" xr2:uid="{8ADF89E4-4784-024D-9BD6-813E99DC2219}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>book_path</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>main_title</t>
   </si>
@@ -64,15 +61,6 @@
     <t>class_info</t>
   </si>
   <si>
-    <t>5, 6</t>
-  </si>
-  <si>
-    <t>5, 7</t>
-  </si>
-  <si>
-    <t>5, 8</t>
-  </si>
-  <si>
     <t>ya_shitau_do</t>
   </si>
   <si>
@@ -82,13 +70,49 @@
     <t>от_слова</t>
   </si>
   <si>
-    <t>Я считаю\n ДО десяти</t>
-  </si>
-  <si>
-    <t>Гимназия \n для дошколят</t>
-  </si>
-  <si>
-    <t>От звука\n к слову</t>
+    <t>age_or_class</t>
+  </si>
+  <si>
+    <t>лет</t>
+  </si>
+  <si>
+    <t>5–6</t>
+  </si>
+  <si>
+    <t>6–6</t>
+  </si>
+  <si>
+    <t>7–6</t>
+  </si>
+  <si>
+    <t>book_path_1</t>
+  </si>
+  <si>
+    <t>book_path_2</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>ya_shitau_do_2</t>
+  </si>
+  <si>
+    <t>гимназя_2</t>
+  </si>
+  <si>
+    <t>от_слова_2</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Я считаю ДО десяти</t>
+  </si>
+  <si>
+    <t>Гимназия для дошколят</t>
+  </si>
+  <si>
+    <t>От звука к слову</t>
   </si>
 </sst>
 </file>
@@ -449,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9148DA9-97A4-7D41-B897-4F15CB551732}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,72 +486,189 @@
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="H7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>